<commit_message>
refactor 5: Update template in
(cherry picked from commit 5dd823368a120b70b93eb9c7d61b3dccd5d505bb)
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_打刻申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_打刻申請_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Project\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,14 +68,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -96,7 +96,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -331,7 +331,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="4"/>
@@ -385,8 +385,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2819400" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3162300" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -722,8 +722,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3369247" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3778822" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1059,8 +1059,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3927140" y="219075"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4403390" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1396,8 +1396,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4474148" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="5017073" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1733,8 +1733,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032041" y="209550"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5641641" y="209550"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -2435,20 +2435,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">

</xml_diff>

<commit_message>
refactor 5: KAFXXX: Update bug #115671
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_打刻申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_打刻申請_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Project\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEDB6D-85D7-43DA-A262-6EC2A25C55AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060"/>
+    <workbookView xWindow="6240" yWindow="1545" windowWidth="20100" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="打刻申請" sheetId="28" r:id="rId1"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -103,7 +104,7 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="源ノ角ゴシック JP Normal"/>
+      <name val="源ノ角ゴシック Normal"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -287,6 +288,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -299,6 +306,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -308,35 +321,23 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2"/>
-    <cellStyle name="標準 2" xfId="1"/>
-    <cellStyle name="標準 2 2" xfId="4"/>
-    <cellStyle name="標準 3" xfId="3"/>
-    <cellStyle name="標準 3 2 2" xfId="5"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -377,7 +378,7 @@
         <xdr:cNvPr id="142" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E452B42-208F-4E5C-A8BE-47F4DE31B10A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E452B42-208F-4E5C-A8BE-47F4DE31B10A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -396,7 +397,7 @@
           <xdr:cNvPr id="143" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C18BFF7-1D3C-4BEC-83AE-FBB78B4C1E7C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C18BFF7-1D3C-4BEC-83AE-FBB78B4C1E7C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -439,8 +440,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -450,7 +451,7 @@
           <xdr:cNvPr id="144" name="直線コネクタ 143">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0335710-48A7-4AD7-9F29-B0D3F2D46CF9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0335710-48A7-4AD7-9F29-B0D3F2D46CF9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -490,7 +491,7 @@
           <xdr:cNvPr id="145" name="直線コネクタ 144">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF5F488-821E-47E5-8B9A-55CF502579F9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF5F488-821E-47E5-8B9A-55CF502579F9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -530,7 +531,7 @@
           <xdr:cNvPr id="146" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72539C0-F327-41E1-B777-843841ED2FC7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72539C0-F327-41E1-B777-843841ED2FC7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -568,13 +569,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -583,7 +587,7 @@
           <xdr:cNvPr id="147" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442D6A60-AC68-4D7B-81A9-B921AB0572CA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442D6A60-AC68-4D7B-81A9-B921AB0572CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -621,13 +625,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -636,7 +643,7 @@
           <xdr:cNvPr id="148" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DA167D-88A0-46E0-970C-F414BF56F4EA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DA167D-88A0-46E0-970C-F414BF56F4EA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -674,13 +681,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -705,7 +715,7 @@
         <xdr:cNvPr id="149" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDB26F7-7FB0-4E89-AD00-9CD595A50AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDB26F7-7FB0-4E89-AD00-9CD595A50AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -724,7 +734,7 @@
           <xdr:cNvPr id="150" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4BD7E5A-4F32-4053-9054-E09E0E1EB3B7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4BD7E5A-4F32-4053-9054-E09E0E1EB3B7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -767,8 +777,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -778,7 +788,7 @@
           <xdr:cNvPr id="151" name="直線コネクタ 150">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC5A912-AD8E-473D-8215-BD04EBC8C347}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC5A912-AD8E-473D-8215-BD04EBC8C347}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -818,7 +828,7 @@
           <xdr:cNvPr id="152" name="直線コネクタ 151">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D681D7DB-8205-40B8-AD03-E1274E19A731}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D681D7DB-8205-40B8-AD03-E1274E19A731}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -858,7 +868,7 @@
           <xdr:cNvPr id="153" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE9971E1-CAB2-4C10-827C-19AF1E0EC9F6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE9971E1-CAB2-4C10-827C-19AF1E0EC9F6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -896,13 +906,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -911,7 +924,7 @@
           <xdr:cNvPr id="154" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67888F9D-E4DA-413D-8123-760A56E5DB16}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67888F9D-E4DA-413D-8123-760A56E5DB16}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -949,13 +962,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -964,7 +980,7 @@
           <xdr:cNvPr id="155" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE084E5-FA6A-444B-A6A8-48DACC6E26F0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE084E5-FA6A-444B-A6A8-48DACC6E26F0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1002,13 +1018,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1033,7 +1052,7 @@
         <xdr:cNvPr id="156" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C643E8-8149-40F8-A27D-2F7D7AB10C63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C643E8-8149-40F8-A27D-2F7D7AB10C63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1052,7 +1071,7 @@
           <xdr:cNvPr id="157" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A63F798A-5995-443A-B978-AC08DD78263F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A63F798A-5995-443A-B978-AC08DD78263F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1095,8 +1114,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1106,7 +1125,7 @@
           <xdr:cNvPr id="158" name="直線コネクタ 157">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558A009B-86F7-4B3E-94F2-077DCF930724}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558A009B-86F7-4B3E-94F2-077DCF930724}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1146,7 +1165,7 @@
           <xdr:cNvPr id="159" name="直線コネクタ 158">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D85164-817F-45B2-9E33-B64B3B2A2ABF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D85164-817F-45B2-9E33-B64B3B2A2ABF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1186,7 +1205,7 @@
           <xdr:cNvPr id="160" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE38C6B0-9B72-41D8-8ACE-F3DED2D7B4CB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE38C6B0-9B72-41D8-8ACE-F3DED2D7B4CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1224,13 +1243,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1239,7 +1261,7 @@
           <xdr:cNvPr id="161" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF65E661-6027-4B7E-BA82-415ED2880596}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF65E661-6027-4B7E-BA82-415ED2880596}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1277,13 +1299,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1292,7 +1317,7 @@
           <xdr:cNvPr id="162" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F04A39A-0074-468B-8721-DD5D79A0E37C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F04A39A-0074-468B-8721-DD5D79A0E37C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1330,13 +1355,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1361,7 +1389,7 @@
         <xdr:cNvPr id="163" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB18411C-DBCE-42E6-86FC-5414D81705F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB18411C-DBCE-42E6-86FC-5414D81705F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1380,7 +1408,7 @@
           <xdr:cNvPr id="164" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E6F564-1C71-4CFD-BDF2-06B65C7D85BB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E6F564-1C71-4CFD-BDF2-06B65C7D85BB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1423,8 +1451,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1434,7 +1462,7 @@
           <xdr:cNvPr id="165" name="直線コネクタ 164">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944CBE9C-C403-4CDD-AA1D-44772DAD8BD4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944CBE9C-C403-4CDD-AA1D-44772DAD8BD4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1474,7 +1502,7 @@
           <xdr:cNvPr id="166" name="直線コネクタ 165">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B11EA4FF-52C6-4E89-B3BF-F58D0C2FB6FA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B11EA4FF-52C6-4E89-B3BF-F58D0C2FB6FA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1514,7 +1542,7 @@
           <xdr:cNvPr id="167" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E35B450-9799-463E-AB58-A18C26718C0A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E35B450-9799-463E-AB58-A18C26718C0A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1552,13 +1580,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1567,7 +1598,7 @@
           <xdr:cNvPr id="168" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED672590-0A93-4CD0-A135-E2A68E885F07}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED672590-0A93-4CD0-A135-E2A68E885F07}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1605,13 +1636,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1620,7 +1654,7 @@
           <xdr:cNvPr id="169" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34640932-3031-4AEA-8174-5A7CE261E06C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34640932-3031-4AEA-8174-5A7CE261E06C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1658,13 +1692,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1689,7 +1726,7 @@
         <xdr:cNvPr id="170" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{995FB280-7D53-4E08-827C-722197ABB0CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{995FB280-7D53-4E08-827C-722197ABB0CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1708,7 +1745,7 @@
           <xdr:cNvPr id="171" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C414845B-2F24-469F-B383-A27788123D5F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C414845B-2F24-469F-B383-A27788123D5F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1751,8 +1788,8 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1762,7 +1799,7 @@
           <xdr:cNvPr id="172" name="直線コネクタ 171">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E098A3-51EB-43D1-A1F4-EADEFCA249AC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E098A3-51EB-43D1-A1F4-EADEFCA249AC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1802,7 +1839,7 @@
           <xdr:cNvPr id="173" name="直線コネクタ 172">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E93B1E-549E-482E-A3E1-12F04754B7CE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E93B1E-549E-482E-A3E1-12F04754B7CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1842,7 +1879,7 @@
           <xdr:cNvPr id="174" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D2A5E6-BFC2-43D9-A4D8-C0C47F379E4A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D2A5E6-BFC2-43D9-A4D8-C0C47F379E4A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1880,13 +1917,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1895,7 +1935,7 @@
           <xdr:cNvPr id="175" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43267093-2B22-40A3-8DA8-6C2CCF13A32E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43267093-2B22-40A3-8DA8-6C2CCF13A32E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1933,13 +1973,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1948,7 +1991,7 @@
           <xdr:cNvPr id="176" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACB5526-E51A-4F61-88BC-6B7FB256B22D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACB5526-E51A-4F61-88BC-6B7FB256B22D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1986,13 +2029,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2387,12 +2433,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
     <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
@@ -2425,240 +2471,240 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1"/>
     <row r="22" spans="2:11" ht="15" customHeight="1"/>

</xml_diff>